<commit_message>
updated examples from owlplanner
</commit_message>
<xml_diff>
--- a/examples/example01/HFP_jack+jill.xlsx
+++ b/examples/example01/HFP_jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\john\projects\owl-station\examples\example01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdlacasse/Owl/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB16B45-0921-4E83-A23F-D55F2D02D571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD35A25-49E6-9B4A-A20A-9670F53C2694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3970" yWindow="2090" windowWidth="26440" windowHeight="17680" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>year</t>
   </si>
@@ -481,30 +481,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB57614-FCF1-4139-AA0D-31AF55A08D66}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -533,9 +533,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -548,9 +548,9 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -563,9 +563,9 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -578,9 +578,9 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -593,9 +593,9 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>2024</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2025</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -610,9 +610,9 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B7" s="1">
         <v>100000</v>
@@ -627,9 +627,9 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B8" s="1">
         <v>100000</v>
@@ -644,9 +644,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B9" s="1">
         <v>100000</v>
@@ -661,9 +661,9 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -676,9 +676,9 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -689,9 +689,9 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -702,9 +702,9 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -715,9 +715,9 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -728,9 +728,9 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -741,9 +741,9 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -754,9 +754,9 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -767,9 +767,9 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -780,9 +780,9 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -793,9 +793,9 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -806,9 +806,9 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -819,9 +819,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -832,9 +832,9 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -845,9 +845,9 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -858,9 +858,9 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -871,9 +871,9 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -884,9 +884,9 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -897,9 +897,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -910,9 +910,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -923,9 +923,9 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -936,9 +936,9 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -949,9 +949,9 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -962,9 +962,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -975,9 +975,9 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -988,9 +988,9 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1001,9 +1001,9 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1014,11 +1014,6 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>2055</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1027,26 +1022,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE7EE4-731B-47FB-9A4E-667972814602}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1075,9 +1070,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1090,9 +1085,9 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1105,9 +1100,9 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1120,9 +1115,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1135,9 +1130,9 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>2024</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2025</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1150,9 +1145,9 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B7" s="6">
         <v>80000</v>
@@ -1165,9 +1160,9 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B8" s="6">
         <v>80000</v>
@@ -1180,9 +1175,9 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B9" s="6">
         <v>85000</v>
@@ -1195,9 +1190,9 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1208,9 +1203,9 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1221,9 +1216,9 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1234,9 +1229,9 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1247,9 +1242,9 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1260,9 +1255,9 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1273,9 +1268,9 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1286,9 +1281,9 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1299,9 +1294,9 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1312,9 +1307,9 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1325,9 +1320,9 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1338,9 +1333,9 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1351,9 +1346,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1364,9 +1359,9 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1377,9 +1372,9 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1390,9 +1385,9 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1403,9 +1398,9 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1416,9 +1411,9 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1429,9 +1424,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1442,9 +1437,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1455,9 +1450,9 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1468,9 +1463,9 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1481,9 +1476,9 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1494,9 +1489,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1507,9 +1502,9 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1520,9 +1515,9 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1533,9 +1528,9 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1546,9 +1541,9 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1559,9 +1554,9 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1572,13 +1567,8 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40">
         <v>2058</v>
       </c>
     </row>
@@ -1592,21 +1582,21 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="1"/>
-    <col min="7" max="7" width="10.26953125" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" customWidth="1"/>
+    <col min="1" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1636,22 +1626,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29335860-5C91-4189-B35F-4DDEB06D1DBA}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1661,19 +1652,22 @@
       <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>